<commit_message>
EPP Variable Installments T2 scenarios
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2479-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-DL-MD-TR-2-PATTERN-VAR-INST-PERIODIC-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/2479-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-DL-MD-TR-2-PATTERN-VAR-INST-PERIODIC-Makerepayment1.xlsx
@@ -213,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -227,9 +227,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -561,7 +558,7 @@
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>42037</v>
       </c>
     </row>
@@ -573,10 +570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +587,7 @@
     <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -610,27 +607,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>5000</v>
       </c>
       <c r="B2" s="6">
-        <v>848.21</v>
+        <v>900</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6">
         <v>0</v>
       </c>
-      <c r="E2" s="9">
-        <v>4151.79</v>
+      <c r="E2" s="8">
+        <v>4100</v>
       </c>
       <c r="F2" s="6">
-        <v>858.48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>900</v>
+      </c>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>181.28</v>
+        <v>175.54</v>
       </c>
       <c r="B3" s="6">
         <v>51.79</v>
@@ -642,13 +640,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>129.49</v>
+        <v>123.75</v>
       </c>
       <c r="F3" s="6">
-        <v>41.52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -668,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>0</v>
       </c>
@@ -698,7 +696,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,7 +794,7 @@
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
-      <c r="P2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -811,12 +809,12 @@
       <c r="D3" s="7">
         <v>42037</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="6">
-        <v>848.21</v>
-      </c>
-      <c r="G3" s="9">
-        <v>4151.79</v>
+        <v>900</v>
+      </c>
+      <c r="G3" s="8">
+        <v>4100</v>
       </c>
       <c r="H3" s="6">
         <v>51.79</v>
@@ -828,10 +826,10 @@
         <v>0</v>
       </c>
       <c r="K3" s="6">
-        <v>900</v>
+        <v>951.79</v>
       </c>
       <c r="L3" s="6">
-        <v>900</v>
+        <v>951.79</v>
       </c>
       <c r="M3" s="6">
         <v>0</v>
@@ -856,13 +854,13 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6">
-        <v>858.48</v>
-      </c>
-      <c r="G4" s="9">
-        <v>3293.31</v>
+        <v>900</v>
+      </c>
+      <c r="G4" s="8">
+        <v>3200</v>
       </c>
       <c r="H4" s="6">
-        <v>41.52</v>
+        <v>41</v>
       </c>
       <c r="I4" s="6">
         <v>0</v>
@@ -871,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="6">
-        <v>900</v>
+        <v>941</v>
       </c>
       <c r="L4" s="6">
         <v>0</v>
@@ -883,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="6">
-        <v>900</v>
+        <v>941</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -899,13 +897,13 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6">
-        <v>858.72</v>
-      </c>
-      <c r="G5" s="9">
-        <v>2434.59</v>
+        <v>900</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2300</v>
       </c>
       <c r="H5" s="6">
-        <v>41.28</v>
+        <v>40.75</v>
       </c>
       <c r="I5" s="6">
         <v>0</v>
@@ -914,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="6">
-        <v>900</v>
+        <v>940.75</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -926,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="6">
-        <v>900</v>
+        <v>940.75</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -942,13 +940,13 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6">
-        <v>875.65</v>
-      </c>
-      <c r="G6" s="9">
-        <v>1558.94</v>
+        <v>900</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1400</v>
       </c>
       <c r="H6" s="6">
-        <v>24.35</v>
+        <v>23</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
@@ -957,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="6">
-        <v>900</v>
+        <v>923</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -969,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="6">
-        <v>900</v>
+        <v>923</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -985,13 +983,13 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6">
-        <v>884.41</v>
+        <v>900</v>
       </c>
       <c r="G7" s="6">
-        <v>674.53</v>
+        <v>500</v>
       </c>
       <c r="H7" s="6">
-        <v>15.59</v>
+        <v>14</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
@@ -1000,7 +998,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="6">
-        <v>900</v>
+        <v>914</v>
       </c>
       <c r="L7" s="6">
         <v>0</v>
@@ -1012,7 +1010,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="6">
-        <v>900</v>
+        <v>914</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1028,13 +1026,13 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6">
-        <v>674.53</v>
+        <v>500</v>
       </c>
       <c r="G8" s="6">
         <v>0</v>
       </c>
       <c r="H8" s="6">
-        <v>6.75</v>
+        <v>5</v>
       </c>
       <c r="I8" s="6">
         <v>0</v>
@@ -1043,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="6">
-        <v>681.28</v>
+        <v>505</v>
       </c>
       <c r="L8" s="6">
         <v>0</v>
@@ -1055,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="6">
-        <v>681.28</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -1069,7 +1067,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,7 +1119,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>53</v>
+        <v>3562</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>27</v>
@@ -1133,10 +1131,10 @@
         <v>31</v>
       </c>
       <c r="E2" s="6">
+        <v>951.79</v>
+      </c>
+      <c r="F2" s="6">
         <v>900</v>
-      </c>
-      <c r="F2" s="6">
-        <v>848.21</v>
       </c>
       <c r="G2" s="6">
         <v>51.79</v>
@@ -1147,15 +1145,15 @@
       <c r="I2" s="6">
         <v>0</v>
       </c>
-      <c r="J2" s="9">
-        <v>4151.79</v>
-      </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="J2" s="8">
+        <v>4100</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>52</v>
+        <v>3557</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>27</v>

</xml_diff>